<commit_message>
reorganized everything and reached a finalized SOP for AIT
</commit_message>
<xml_diff>
--- a/docs/SOP/Signatures.xlsx
+++ b/docs/SOP/Signatures.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\AIT\experimental_setup\sop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\AIT\experimental_setup\ait_exp\docs\SOP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -38,13 +38,14 @@
     <t xml:space="preserve">AIT SOP SIGNATURES </t>
   </si>
   <si>
-    <t xml:space="preserve"> SOP revision date:                                </t>
-  </si>
-  <si>
     <t>By signing this, I assert that I have:
 - Completed pertient laboratory safety training
 - Read the AIT SOP in its entirety
-- Become familiar with all the experimental steps outlined in the AIT SOP</t>
+- Become familiar with all the experimental steps outlined in the AIT SOP
+- Sufficient competence to complete these experiments safely</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SOP revision date:  July 30, 2018 </t>
   </si>
 </sst>
 </file>
@@ -404,7 +405,7 @@
   <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A3" sqref="A3:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,14 +430,14 @@
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -613,6 +614,6 @@
     <mergeCell ref="C2:E2"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="79" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="76" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>